<commit_message>
Code cleanup, todo updated
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16571" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16573" uniqueCount="190">
   <si>
     <t>Change table design to match table-design.png</t>
   </si>
@@ -665,6 +665,12 @@
   <si>
     <t>Translation and glossary detail pages, add "Download" button (various formats such as as Word file, excel file, text file).</t>
   </si>
+  <si>
+    <t>Have two basic user accounts, honyakubu and non-honyakubu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Non-honyakubu can only see PCT translations (add a PCT-flag to the translation model?)</t>
+  </si>
 </sst>
 </file>
 
@@ -1079,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD188"/>
+  <dimension ref="A1:XFD190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -67371,7 +67377,7 @@
       </c>
     </row>
     <row r="150" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="8" t="s">
         <v>84</v>
       </c>
     </row>
@@ -67563,6 +67569,16 @@
     <row r="188" spans="1:1" ht="20.100000000000001" customHeight="1">
       <c r="A188" s="2" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A189" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A190" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Template table cell icon update
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16575" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16576" uniqueCount="193">
   <si>
     <t>Change table design to match table-design.png</t>
   </si>
@@ -677,6 +677,9 @@
   <si>
     <t>BUG - last resource not selected on dropdown menu when viewing form pages (only being selected on search result page)</t>
   </si>
+  <si>
+    <t>BUG - when copy to clipboard item clicked in table, don’t move to search bar (instead display tooltip "copied")</t>
+  </si>
 </sst>
 </file>
 
@@ -1091,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD192"/>
+  <dimension ref="A1:XFD193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A193" sqref="A193"/>
+      <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -67597,6 +67600,11 @@
         <v>191</v>
       </c>
     </row>
+    <row r="193" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A193" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug fix in glossary Item form
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16576" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16580" uniqueCount="197">
   <si>
     <t>Change table design to match table-design.png</t>
   </si>
@@ -680,6 +680,18 @@
   <si>
     <t>BUG - last resource not selected on dropdown menu when viewing form pages (only being selected on search result page) = just use modals?</t>
   </si>
+  <si>
+    <t>BUG - in the entry create/update form, the list of glossaries provided includes all resources not just glossaries</t>
+  </si>
+  <si>
+    <t>BUG - the size of the monster glossary is a problem, particularly when redirecting thereto after creating a new entry therefor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           - only show the first 100 entries (and include warning of there are lots of entries)</t>
+  </si>
+  <si>
+    <t>Include links to reorder the resource content table (similar to the homepage table)</t>
+  </si>
 </sst>
 </file>
 
@@ -782,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -813,6 +825,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1094,9 +1112,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD193"/>
+  <dimension ref="A1:XFD197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
       <selection activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
@@ -67605,6 +67623,26 @@
         <v>191</v>
       </c>
     </row>
+    <row r="194" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A194" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A195" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A196" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="20.100000000000001" customHeight="1">
+      <c r="A197" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
File renamed, todo updated
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1121,7 +1121,7 @@
   <dimension ref="A1:XFD199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A194" sqref="A194"/>
+      <selection activeCell="A192" sqref="A192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -67650,12 +67650,12 @@
       </c>
     </row>
     <row r="198" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A198" s="5" t="s">
+      <c r="A198" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="20.100000000000001" customHeight="1">
-      <c r="A199" s="5" t="s">
+      <c r="A199" s="9" t="s">
         <v>198</v>
       </c>
     </row>

</xml_diff>